<commit_message>
Psensor can now also median temperature and standard deviation. Modified notebook to be able to show t medias on plot.
</commit_message>
<xml_diff>
--- a/docs/Examples/Example6_esitec_pressure_calibration/merged_dataframe.xlsx
+++ b/docs/Examples/Example6_esitec_pressure_calibration/merged_dataframe.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="401" uniqueCount="182">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="403" uniqueCount="184">
   <si>
     <t>filename_x</t>
   </si>
@@ -191,6 +191,12 @@
   </si>
   <si>
     <t>mad_pressure</t>
+  </si>
+  <si>
+    <t>median_temp</t>
+  </si>
+  <si>
+    <t>mad_temp</t>
   </si>
   <si>
     <t>FDCA1</t>
@@ -921,13 +927,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:BH39"/>
+  <dimension ref="A1:BJ39"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:60">
+    <row r="1" spans="1:62">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1105,13 +1111,19 @@
       <c r="BH1" s="1" t="s">
         <v>58</v>
       </c>
+      <c r="BI1" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="BJ1" s="1" t="s">
+        <v>60</v>
+      </c>
     </row>
-    <row r="2" spans="1:60">
+    <row r="2" spans="1:62">
       <c r="A2" s="1">
         <v>29</v>
       </c>
       <c r="B2" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="C2">
         <v>104.9329632313256</v>
@@ -1144,7 +1156,7 @@
         <v>2.004071642835179</v>
       </c>
       <c r="M2" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="N2">
         <v>1385.900154457914</v>
@@ -1171,7 +1183,7 @@
         <v>1.935568023656017</v>
       </c>
       <c r="W2" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="X2">
         <v>1260.917536643933</v>
@@ -1219,16 +1231,16 @@
         <v>13.90021244502253</v>
       </c>
       <c r="AM2" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="AN2" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="AO2" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="AP2" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="AQ2">
         <v>27</v>
@@ -1243,10 +1255,10 @@
         <v>5</v>
       </c>
       <c r="AV2" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="AW2" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="AX2">
         <v>61904</v>
@@ -1281,13 +1293,19 @@
       <c r="BH2">
         <v>0.0007095336914066941</v>
       </c>
+      <c r="BI2">
+        <v>32.01123046875</v>
+      </c>
+      <c r="BJ2">
+        <v>0.0015869140625</v>
+      </c>
     </row>
-    <row r="3" spans="1:60">
+    <row r="3" spans="1:62">
       <c r="A3" s="1">
         <v>30</v>
       </c>
       <c r="B3" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="C3">
         <v>104.9396743499796</v>
@@ -1320,7 +1338,7 @@
         <v>2.005432771511782</v>
       </c>
       <c r="M3" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="N3">
         <v>1385.902077914185</v>
@@ -1347,7 +1365,7 @@
         <v>1.938074842235596</v>
       </c>
       <c r="W3" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="X3">
         <v>1260.91464331601</v>
@@ -1395,16 +1413,16 @@
         <v>12.40094081348089</v>
       </c>
       <c r="AM3" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="AN3" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="AO3" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="AP3" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="AQ3">
         <v>27</v>
@@ -1419,10 +1437,10 @@
         <v>5</v>
       </c>
       <c r="AV3" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="AW3" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="AX3">
         <v>62097</v>
@@ -1457,13 +1475,19 @@
       <c r="BH3">
         <v>0.0006814360618592197</v>
       </c>
+      <c r="BI3">
+        <v>32.03125</v>
+      </c>
+      <c r="BJ3">
+        <v>0.001035690307617188</v>
+      </c>
     </row>
-    <row r="4" spans="1:60">
+    <row r="4" spans="1:62">
       <c r="A4" s="1">
         <v>31</v>
       </c>
       <c r="B4" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="C4">
         <v>104.9413011430268</v>
@@ -1496,7 +1520,7 @@
         <v>2.013054972251721</v>
       </c>
       <c r="M4" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="N4">
         <v>1385.905417387628</v>
@@ -1523,7 +1547,7 @@
         <v>1.935744220425104</v>
       </c>
       <c r="W4" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="X4">
         <v>1260.886305434603</v>
@@ -1571,16 +1595,16 @@
         <v>13.25914925713328</v>
       </c>
       <c r="AM4" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="AN4" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="AO4" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="AP4" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="AQ4">
         <v>27</v>
@@ -1595,10 +1619,10 @@
         <v>5</v>
       </c>
       <c r="AV4" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="AW4" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="AX4">
         <v>62312</v>
@@ -1633,13 +1657,19 @@
       <c r="BH4">
         <v>0.0007912755012504658</v>
       </c>
+      <c r="BI4">
+        <v>32.0458984375</v>
+      </c>
+      <c r="BJ4">
+        <v>0.001071929931640625</v>
+      </c>
     </row>
-    <row r="5" spans="1:60">
+    <row r="5" spans="1:62">
       <c r="A5" s="1">
         <v>32</v>
       </c>
       <c r="B5" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="C5">
         <v>104.6903523224214</v>
@@ -1672,7 +1702,7 @@
         <v>2.007644142983221</v>
       </c>
       <c r="M5" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="N5">
         <v>1386.090522788008</v>
@@ -1699,7 +1729,7 @@
         <v>1.888706114395819</v>
       </c>
       <c r="W5" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="X5">
         <v>1261.348945353441</v>
@@ -1747,16 +1777,16 @@
         <v>14.0925281340322</v>
       </c>
       <c r="AM5" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="AN5" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="AO5" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="AP5" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="AQ5">
         <v>27</v>
@@ -1771,10 +1801,10 @@
         <v>5</v>
       </c>
       <c r="AV5" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="AW5" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="AX5">
         <v>62804</v>
@@ -1809,13 +1839,19 @@
       <c r="BH5">
         <v>0.0004417419433594416</v>
       </c>
+      <c r="BI5">
+        <v>32.0458984375</v>
+      </c>
+      <c r="BJ5">
+        <v>0.00136566162109375</v>
+      </c>
     </row>
-    <row r="6" spans="1:60">
+    <row r="6" spans="1:62">
       <c r="A6" s="1">
         <v>33</v>
       </c>
       <c r="B6" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="C6">
         <v>104.6818475429104</v>
@@ -1848,7 +1884,7 @@
         <v>2.00569594216536</v>
       </c>
       <c r="M6" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="N6">
         <v>1386.086671295273</v>
@@ -1875,7 +1911,7 @@
         <v>1.882908729450017</v>
       </c>
       <c r="W6" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="X6">
         <v>1261.418383797672</v>
@@ -1923,16 +1959,16 @@
         <v>14.3677588677225</v>
       </c>
       <c r="AM6" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="AN6" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="AO6" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="AP6" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="AQ6">
         <v>27</v>
@@ -1947,10 +1983,10 @@
         <v>5</v>
       </c>
       <c r="AV6" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="AW6" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="AX6">
         <v>63045</v>
@@ -1985,13 +2021,19 @@
       <c r="BH6">
         <v>0.00067093372344873</v>
       </c>
+      <c r="BI6">
+        <v>32.072265625</v>
+      </c>
+      <c r="BJ6">
+        <v>0.001230239868164062</v>
+      </c>
     </row>
-    <row r="7" spans="1:60">
+    <row r="7" spans="1:62">
       <c r="A7" s="1">
         <v>34</v>
       </c>
       <c r="B7" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="C7">
         <v>104.688591793962</v>
@@ -2024,7 +2066,7 @@
         <v>1.987481600059859</v>
       </c>
       <c r="M7" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="N7">
         <v>1386.087162078147</v>
@@ -2051,7 +2093,7 @@
         <v>1.874870368914806</v>
       </c>
       <c r="W7" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="X7">
         <v>1261.346650016464</v>
@@ -2099,16 +2141,16 @@
         <v>13.63362920958058</v>
       </c>
       <c r="AM7" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="AN7" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="AO7" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="AP7" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="AQ7">
         <v>27</v>
@@ -2123,10 +2165,10 @@
         <v>5</v>
       </c>
       <c r="AV7" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="AW7" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="AX7">
         <v>63235</v>
@@ -2161,13 +2203,19 @@
       <c r="BH7">
         <v>0.0006076097488416643</v>
       </c>
+      <c r="BI7">
+        <v>32.08984375</v>
+      </c>
+      <c r="BJ7">
+        <v>0.00092315673828125</v>
+      </c>
     </row>
-    <row r="8" spans="1:60">
+    <row r="8" spans="1:62">
       <c r="A8" s="1">
         <v>35</v>
       </c>
       <c r="B8" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="C8">
         <v>104.3707700556391</v>
@@ -2200,7 +2248,7 @@
         <v>2.117588022702473</v>
       </c>
       <c r="M8" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="N8">
         <v>1386.399704168115</v>
@@ -2227,7 +2275,7 @@
         <v>1.80705694272221</v>
       </c>
       <c r="W8" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="X8">
         <v>1261.942148647291</v>
@@ -2275,16 +2323,16 @@
         <v>17.86266911157816</v>
       </c>
       <c r="AM8" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="AN8" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="AO8" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="AP8" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="AQ8">
         <v>27</v>
@@ -2299,10 +2347,10 @@
         <v>5</v>
       </c>
       <c r="AV8" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="AW8" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="AX8">
         <v>63917</v>
@@ -2337,13 +2385,19 @@
       <c r="BH8">
         <v>0.0004800856113431062</v>
       </c>
+      <c r="BI8">
+        <v>32.1611328125</v>
+      </c>
+      <c r="BJ8">
+        <v>0.001279830932617188</v>
+      </c>
     </row>
-    <row r="9" spans="1:60">
+    <row r="9" spans="1:62">
       <c r="A9" s="1">
         <v>36</v>
       </c>
       <c r="B9" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="C9">
         <v>104.3792014029755</v>
@@ -2376,7 +2430,7 @@
         <v>2.114824819340348</v>
       </c>
       <c r="M9" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="N9">
         <v>1386.403696228714</v>
@@ -2403,7 +2457,7 @@
         <v>1.813452898226622</v>
       </c>
       <c r="W9" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="X9">
         <v>1262.005643892569</v>
@@ -2451,16 +2505,16 @@
         <v>17.20630133125116</v>
       </c>
       <c r="AM9" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="AN9" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="AO9" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="AP9" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="AQ9">
         <v>27</v>
@@ -2475,10 +2529,10 @@
         <v>5</v>
       </c>
       <c r="AV9" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="AW9" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="AX9">
         <v>64106</v>
@@ -2513,13 +2567,19 @@
       <c r="BH9">
         <v>0.0006869688630105064</v>
       </c>
+      <c r="BI9">
+        <v>32.1875</v>
+      </c>
+      <c r="BJ9">
+        <v>0.00160980224609375</v>
+      </c>
     </row>
-    <row r="10" spans="1:60">
+    <row r="10" spans="1:62">
       <c r="A10" s="1">
         <v>37</v>
       </c>
       <c r="B10" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="C10">
         <v>104.3748173295075</v>
@@ -2552,7 +2612,7 @@
         <v>2.098587500528921</v>
       </c>
       <c r="M10" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="N10">
         <v>1386.403230956724</v>
@@ -2579,7 +2639,7 @@
         <v>1.799718907888751</v>
       </c>
       <c r="W10" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="X10">
         <v>1262.026575433455</v>
@@ -2627,16 +2687,16 @@
         <v>18.16227391253155</v>
       </c>
       <c r="AM10" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="AN10" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="AO10" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="AP10" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="AQ10">
         <v>27</v>
@@ -2651,10 +2711,10 @@
         <v>5</v>
       </c>
       <c r="AV10" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="AW10" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="AX10">
         <v>64742</v>
@@ -2689,13 +2749,19 @@
       <c r="BH10">
         <v>0.0006322950124737492</v>
       </c>
+      <c r="BI10">
+        <v>32.2158203125</v>
+      </c>
+      <c r="BJ10">
+        <v>0.0006694793701171875</v>
+      </c>
     </row>
-    <row r="11" spans="1:60">
+    <row r="11" spans="1:62">
       <c r="A11" s="1">
         <v>6</v>
       </c>
       <c r="B11" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="C11">
         <v>104.1276251189742</v>
@@ -2728,7 +2794,7 @@
         <v>2.251772501139534</v>
       </c>
       <c r="M11" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="N11">
         <v>1386.651046648162</v>
@@ -2755,7 +2821,7 @@
         <v>1.802238613981302</v>
       </c>
       <c r="W11" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="X11">
         <v>1262.515294360687</v>
@@ -2794,16 +2860,16 @@
         <v>21.0942298094733</v>
       </c>
       <c r="AM11" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="AN11" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="AO11" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="AP11" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="AQ11">
         <v>27</v>
@@ -2818,10 +2884,10 @@
         <v>5</v>
       </c>
       <c r="AV11" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="AW11" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="AX11">
         <v>67635</v>
@@ -2856,13 +2922,19 @@
       <c r="BH11">
         <v>0.0005644083023067514</v>
       </c>
+      <c r="BI11">
+        <v>32.5439453125</v>
+      </c>
+      <c r="BJ11">
+        <v>0.001209259033203125</v>
+      </c>
     </row>
-    <row r="12" spans="1:60">
+    <row r="12" spans="1:62">
       <c r="A12" s="1">
         <v>7</v>
       </c>
       <c r="B12" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="C12">
         <v>104.1527523207513</v>
@@ -2895,7 +2967,7 @@
         <v>2.271950148515839</v>
       </c>
       <c r="M12" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="N12">
         <v>1386.658480414131</v>
@@ -2922,7 +2994,7 @@
         <v>1.817923073958469</v>
       </c>
       <c r="W12" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="X12">
         <v>1262.601146524149</v>
@@ -2961,16 +3033,16 @@
         <v>20.55299115861916</v>
       </c>
       <c r="AM12" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="AN12" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="AO12" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="AP12" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="AQ12">
         <v>27</v>
@@ -2985,10 +3057,10 @@
         <v>5</v>
       </c>
       <c r="AV12" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="AW12" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="AX12">
         <v>67839</v>
@@ -3023,13 +3095,19 @@
       <c r="BH12">
         <v>0.0007705748081209829</v>
       </c>
+      <c r="BI12">
+        <v>32.5576171875</v>
+      </c>
+      <c r="BJ12">
+        <v>0.0009918212890625</v>
+      </c>
     </row>
-    <row r="13" spans="1:60">
+    <row r="13" spans="1:62">
       <c r="A13" s="1">
         <v>8</v>
       </c>
       <c r="B13" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="C13">
         <v>104.1494260305549</v>
@@ -3062,7 +3140,7 @@
         <v>2.267415917653915</v>
       </c>
       <c r="M13" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="N13">
         <v>1386.660892350618</v>
@@ -3089,7 +3167,7 @@
         <v>1.792877708965141</v>
       </c>
       <c r="W13" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="X13">
         <v>1262.549864828809</v>
@@ -3128,16 +3206,16 @@
         <v>20.05072033535419</v>
       </c>
       <c r="AM13" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="AN13" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="AO13" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="AP13" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="AQ13">
         <v>27</v>
@@ -3152,10 +3230,10 @@
         <v>5</v>
       </c>
       <c r="AV13" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="AW13" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="AX13">
         <v>68074</v>
@@ -3190,13 +3268,19 @@
       <c r="BH13">
         <v>0.0005924358963966814</v>
       </c>
+      <c r="BI13">
+        <v>32.5556640625</v>
+      </c>
+      <c r="BJ13">
+        <v>0.0006256103515625</v>
+      </c>
     </row>
-    <row r="14" spans="1:60">
+    <row r="14" spans="1:62">
       <c r="A14" s="1">
         <v>9</v>
       </c>
       <c r="B14" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="C14">
         <v>104.0201143916676</v>
@@ -3229,7 +3313,7 @@
         <v>2.359575674852487</v>
       </c>
       <c r="M14" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="N14">
         <v>1386.816001775505</v>
@@ -3256,7 +3340,7 @@
         <v>1.822144996265706</v>
       </c>
       <c r="W14" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="X14">
         <v>1262.852554310655</v>
@@ -3295,16 +3379,16 @@
         <v>21.87095913140476</v>
       </c>
       <c r="AM14" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="AN14" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="AO14" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="AP14" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="AQ14">
         <v>27</v>
@@ -3319,10 +3403,10 @@
         <v>5</v>
       </c>
       <c r="AV14" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="AW14" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="AX14">
         <v>68534</v>
@@ -3357,13 +3441,19 @@
       <c r="BH14">
         <v>0.0003698468208311878</v>
       </c>
+      <c r="BI14">
+        <v>32.6796875</v>
+      </c>
+      <c r="BJ14">
+        <v>0.002063751220703125</v>
+      </c>
     </row>
-    <row r="15" spans="1:60">
+    <row r="15" spans="1:62">
       <c r="A15" s="1">
         <v>10</v>
       </c>
       <c r="B15" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="C15">
         <v>104.0020590566906</v>
@@ -3396,7 +3486,7 @@
         <v>2.370235011750542</v>
       </c>
       <c r="M15" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="N15">
         <v>1386.814214167779</v>
@@ -3423,7 +3513,7 @@
         <v>1.791184451267803</v>
       </c>
       <c r="W15" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="X15">
         <v>1262.91959140726</v>
@@ -3462,16 +3552,16 @@
         <v>21.55267375975374</v>
       </c>
       <c r="AM15" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="AN15" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="AO15" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="AP15" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="AQ15">
         <v>27</v>
@@ -3486,10 +3576,10 @@
         <v>5</v>
       </c>
       <c r="AV15" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="AW15" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="AX15">
         <v>68732</v>
@@ -3524,13 +3614,19 @@
       <c r="BH15">
         <v>0.0004374265670776811</v>
       </c>
+      <c r="BI15">
+        <v>32.7216796875</v>
+      </c>
+      <c r="BJ15">
+        <v>0.00153350830078125</v>
+      </c>
     </row>
-    <row r="16" spans="1:60">
+    <row r="16" spans="1:62">
       <c r="A16" s="1">
         <v>11</v>
       </c>
       <c r="B16" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="C16">
         <v>104.020769636694</v>
@@ -3563,7 +3659,7 @@
         <v>2.364657137045858</v>
       </c>
       <c r="M16" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="N16">
         <v>1386.813736300869</v>
@@ -3590,7 +3686,7 @@
         <v>1.782707597004099</v>
       </c>
       <c r="W16" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="X16">
         <v>1262.720216011314</v>
@@ -3629,16 +3725,16 @@
         <v>22.14495994759985</v>
       </c>
       <c r="AM16" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="AN16" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="AO16" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="AP16" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="AQ16">
         <v>27</v>
@@ -3653,10 +3749,10 @@
         <v>5</v>
       </c>
       <c r="AV16" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="AW16" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="AX16">
         <v>68976</v>
@@ -3691,13 +3787,19 @@
       <c r="BH16">
         <v>0.0005769167393035508</v>
       </c>
+      <c r="BI16">
+        <v>32.7509765625</v>
+      </c>
+      <c r="BJ16">
+        <v>0.001036644857668042</v>
+      </c>
     </row>
-    <row r="17" spans="1:60">
+    <row r="17" spans="1:62">
       <c r="A17" s="1">
         <v>12</v>
       </c>
       <c r="B17" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="C17">
         <v>103.8511875436995</v>
@@ -3730,7 +3832,7 @@
         <v>2.45192463134291</v>
       </c>
       <c r="M17" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="N17">
         <v>1387.004489011625</v>
@@ -3757,7 +3859,7 @@
         <v>1.772892938229694</v>
       </c>
       <c r="W17" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="X17">
         <v>1263.148721862417</v>
@@ -3796,16 +3898,16 @@
         <v>22.04821280833813</v>
       </c>
       <c r="AM17" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="AN17" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="AO17" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="AP17" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="AQ17">
         <v>27</v>
@@ -3820,10 +3922,10 @@
         <v>5</v>
       </c>
       <c r="AV17" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="AW17" t="s">
-        <v>159</v>
+        <v>161</v>
       </c>
       <c r="AX17">
         <v>69877</v>
@@ -3858,13 +3960,19 @@
       <c r="BH17">
         <v>0.0006004303693771251</v>
       </c>
+      <c r="BI17">
+        <v>32.890625</v>
+      </c>
+      <c r="BJ17">
+        <v>0.00147247314453125</v>
+      </c>
     </row>
-    <row r="18" spans="1:60">
+    <row r="18" spans="1:62">
       <c r="A18" s="1">
         <v>13</v>
       </c>
       <c r="B18" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="C18">
         <v>103.8497182672101</v>
@@ -3897,7 +4005,7 @@
         <v>2.393617716718523</v>
       </c>
       <c r="M18" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="N18">
         <v>1387.003200954595</v>
@@ -3924,7 +4032,7 @@
         <v>1.782583724836281</v>
       </c>
       <c r="W18" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="X18">
         <v>1263.192765753056</v>
@@ -3963,16 +4071,16 @@
         <v>22.20023762129644</v>
       </c>
       <c r="AM18" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="AN18" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="AO18" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="AP18" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="AQ18">
         <v>27</v>
@@ -3987,10 +4095,10 @@
         <v>5</v>
       </c>
       <c r="AV18" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="AW18" t="s">
-        <v>160</v>
+        <v>162</v>
       </c>
       <c r="AX18">
         <v>70085</v>
@@ -4025,13 +4133,19 @@
       <c r="BH18">
         <v>0.0004320437148470568</v>
       </c>
+      <c r="BI18">
+        <v>32.91796875</v>
+      </c>
+      <c r="BJ18">
+        <v>0.001129907024793114</v>
+      </c>
     </row>
-    <row r="19" spans="1:60">
+    <row r="19" spans="1:62">
       <c r="A19" s="1">
         <v>14</v>
       </c>
       <c r="B19" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="C19">
         <v>103.8441949508049</v>
@@ -4064,7 +4178,7 @@
         <v>2.398517262486756</v>
       </c>
       <c r="M19" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="N19">
         <v>1387.006111651629</v>
@@ -4091,7 +4205,7 @@
         <v>1.808118231527136</v>
       </c>
       <c r="W19" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="X19">
         <v>1263.068893849289</v>
@@ -4130,16 +4244,16 @@
         <v>20.88152931889078</v>
       </c>
       <c r="AM19" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="AN19" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="AO19" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="AP19" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="AQ19">
         <v>27</v>
@@ -4154,10 +4268,10 @@
         <v>5</v>
       </c>
       <c r="AV19" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="AW19" t="s">
-        <v>161</v>
+        <v>163</v>
       </c>
       <c r="AX19">
         <v>70327</v>
@@ -4192,13 +4306,19 @@
       <c r="BH19">
         <v>0.0007356524467465597</v>
       </c>
+      <c r="BI19">
+        <v>32.93359375</v>
+      </c>
+      <c r="BJ19">
+        <v>0.0008640289306640625</v>
+      </c>
     </row>
-    <row r="20" spans="1:60">
+    <row r="20" spans="1:62">
       <c r="A20" s="1">
         <v>15</v>
       </c>
       <c r="B20" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="C20">
         <v>103.6498976267414</v>
@@ -4231,7 +4351,7 @@
         <v>2.263991019060115</v>
       </c>
       <c r="M20" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="N20">
         <v>1387.264847445783</v>
@@ -4258,7 +4378,7 @@
         <v>1.697877238623187</v>
       </c>
       <c r="W20" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="AA20">
         <v>1408.667187406486</v>
@@ -4288,16 +4408,16 @@
         <v>21.16787551990861</v>
       </c>
       <c r="AM20" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="AN20" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="AO20" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="AP20" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="AQ20">
         <v>27</v>
@@ -4312,10 +4432,10 @@
         <v>5</v>
       </c>
       <c r="AV20" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="AW20" t="s">
-        <v>162</v>
+        <v>164</v>
       </c>
       <c r="AX20">
         <v>71068</v>
@@ -4350,13 +4470,19 @@
       <c r="BH20">
         <v>0.0005061904679268719</v>
       </c>
+      <c r="BI20">
+        <v>32.92578125</v>
+      </c>
+      <c r="BJ20">
+        <v>0.000962857910819446</v>
+      </c>
     </row>
-    <row r="21" spans="1:60">
+    <row r="21" spans="1:62">
       <c r="A21" s="1">
         <v>16</v>
       </c>
       <c r="B21" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="C21">
         <v>103.6564583567969</v>
@@ -4389,7 +4515,7 @@
         <v>2.315063218956265</v>
       </c>
       <c r="M21" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="N21">
         <v>1387.265624591877</v>
@@ -4416,7 +4542,7 @@
         <v>1.699190159018645</v>
       </c>
       <c r="W21" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="X21">
         <v>1263.575457887308</v>
@@ -4446,16 +4572,16 @@
         <v>21.18763645373843</v>
       </c>
       <c r="AM21" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="AN21" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="AO21" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="AP21" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="AQ21">
         <v>27</v>
@@ -4470,10 +4596,10 @@
         <v>5</v>
       </c>
       <c r="AV21" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="AW21" t="s">
-        <v>163</v>
+        <v>165</v>
       </c>
       <c r="AX21">
         <v>71344</v>
@@ -4508,13 +4634,19 @@
       <c r="BH21">
         <v>0.0006228245346185249</v>
       </c>
+      <c r="BI21">
+        <v>32.9345703125</v>
+      </c>
+      <c r="BJ21">
+        <v>0.0009398695676772962</v>
+      </c>
     </row>
-    <row r="22" spans="1:60">
+    <row r="22" spans="1:62">
       <c r="A22" s="1">
         <v>17</v>
       </c>
       <c r="B22" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="C22">
         <v>103.6618676346246</v>
@@ -4547,7 +4679,7 @@
         <v>2.267320683162311</v>
       </c>
       <c r="M22" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="N22">
         <v>1387.267578053549</v>
@@ -4574,7 +4706,7 @@
         <v>1.733787506856976</v>
       </c>
       <c r="W22" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="X22">
         <v>1263.550082868913</v>
@@ -4613,16 +4745,16 @@
         <v>21.61421942542815</v>
       </c>
       <c r="AM22" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="AN22" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="AO22" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="AP22" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="AQ22">
         <v>27</v>
@@ -4637,10 +4769,10 @@
         <v>5</v>
       </c>
       <c r="AV22" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="AW22" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="AX22">
         <v>71562</v>
@@ -4675,13 +4807,19 @@
       <c r="BH22">
         <v>0.0007242011937581867</v>
       </c>
+      <c r="BI22">
+        <v>32.94140625</v>
+      </c>
+      <c r="BJ22">
+        <v>0.0008744412064287948</v>
+      </c>
     </row>
-    <row r="23" spans="1:60">
+    <row r="23" spans="1:62">
       <c r="A23" s="1">
         <v>18</v>
       </c>
       <c r="B23" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="C23">
         <v>103.655127694073</v>
@@ -4714,7 +4852,7 @@
         <v>2.230422038026336</v>
       </c>
       <c r="M23" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="N23">
         <v>1387.256929860473</v>
@@ -4741,7 +4879,7 @@
         <v>1.731597799679854</v>
       </c>
       <c r="W23" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="X23">
         <v>1263.558415157285</v>
@@ -4780,16 +4918,16 @@
         <v>21.58913616575977</v>
       </c>
       <c r="AM23" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="AN23" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="AO23" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="AP23" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="AQ23">
         <v>27</v>
@@ -4804,10 +4942,10 @@
         <v>5</v>
       </c>
       <c r="AV23" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="AW23" t="s">
-        <v>165</v>
+        <v>167</v>
       </c>
       <c r="AX23">
         <v>71793</v>
@@ -4842,13 +4980,19 @@
       <c r="BH23">
         <v>0.0005659746659617099</v>
       </c>
+      <c r="BI23">
+        <v>32.94921875</v>
+      </c>
+      <c r="BJ23">
+        <v>0.0008266961860571841</v>
+      </c>
     </row>
-    <row r="24" spans="1:60">
+    <row r="24" spans="1:62">
       <c r="A24" s="1">
         <v>19</v>
       </c>
       <c r="B24" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="C24">
         <v>103.107805049587</v>
@@ -4881,7 +5025,7 @@
         <v>1.484067007887634</v>
       </c>
       <c r="M24" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="N24">
         <v>1387.992677885464</v>
@@ -4908,7 +5052,7 @@
         <v>1.276321625780966</v>
       </c>
       <c r="W24" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="X24">
         <v>1264.723083336703</v>
@@ -4947,16 +5091,16 @@
         <v>15.88058625915921</v>
       </c>
       <c r="AM24" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="AN24" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="AO24" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="AP24" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="AQ24">
         <v>27</v>
@@ -4971,10 +5115,10 @@
         <v>5</v>
       </c>
       <c r="AV24" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="AW24" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="AX24">
         <v>72191</v>
@@ -5009,13 +5153,19 @@
       <c r="BH24">
         <v>0.0003903737301385261</v>
       </c>
+      <c r="BI24">
+        <v>32.5029296875</v>
+      </c>
+      <c r="BJ24">
+        <v>0.01142811849635794</v>
+      </c>
     </row>
-    <row r="25" spans="1:60">
+    <row r="25" spans="1:62">
       <c r="A25" s="1">
         <v>20</v>
       </c>
       <c r="B25" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="C25">
         <v>103.1096883689026</v>
@@ -5048,7 +5198,7 @@
         <v>1.485822963788813</v>
       </c>
       <c r="M25" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="N25">
         <v>1387.998445677258</v>
@@ -5075,7 +5225,7 @@
         <v>1.268109859583802</v>
       </c>
       <c r="W25" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="X25">
         <v>1264.785028008943</v>
@@ -5114,16 +5264,16 @@
         <v>15.78057785338849</v>
       </c>
       <c r="AM25" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="AN25" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="AO25" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="AP25" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="AQ25">
         <v>27</v>
@@ -5138,10 +5288,10 @@
         <v>5</v>
       </c>
       <c r="AV25" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="AW25" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
       <c r="AX25">
         <v>72507</v>
@@ -5176,13 +5326,19 @@
       <c r="BH25">
         <v>0.0003334529690143144</v>
       </c>
+      <c r="BI25">
+        <v>32.34765625</v>
+      </c>
+      <c r="BJ25">
+        <v>0.004897039216961543</v>
+      </c>
     </row>
-    <row r="26" spans="1:60">
+    <row r="26" spans="1:62">
       <c r="A26" s="1">
         <v>21</v>
       </c>
       <c r="B26" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="C26">
         <v>103.0940161055254</v>
@@ -5215,7 +5371,7 @@
         <v>1.487323278351433</v>
       </c>
       <c r="M26" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="N26">
         <v>1387.999591039767</v>
@@ -5242,7 +5398,7 @@
         <v>1.27324058315378</v>
       </c>
       <c r="W26" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="X26">
         <v>1264.768016455383</v>
@@ -5281,16 +5437,16 @@
         <v>15.84670399293321</v>
       </c>
       <c r="AM26" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="AN26" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="AO26" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="AP26" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="AQ26">
         <v>27</v>
@@ -5305,10 +5461,10 @@
         <v>5</v>
       </c>
       <c r="AV26" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="AW26" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="AX26">
         <v>72773</v>
@@ -5343,13 +5499,19 @@
       <c r="BH26">
         <v>0.0003677566155405017</v>
       </c>
+      <c r="BI26">
+        <v>32.287109375</v>
+      </c>
+      <c r="BJ26">
+        <v>0.002666170634920748</v>
+      </c>
     </row>
-    <row r="27" spans="1:60">
+    <row r="27" spans="1:62">
       <c r="A27" s="1">
         <v>22</v>
       </c>
       <c r="B27" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="C27">
         <v>103.1162877389778</v>
@@ -5382,7 +5544,7 @@
         <v>1.468108769466458</v>
       </c>
       <c r="M27" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="N27">
         <v>1388.001413343348</v>
@@ -5409,7 +5571,7 @@
         <v>1.259804836619766</v>
       </c>
       <c r="W27" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="X27">
         <v>1264.693634256725</v>
@@ -5448,16 +5610,16 @@
         <v>15.66867858724883</v>
       </c>
       <c r="AM27" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="AN27" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="AO27" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="AP27" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="AQ27">
         <v>27</v>
@@ -5472,10 +5634,10 @@
         <v>5</v>
       </c>
       <c r="AV27" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="AW27" t="s">
-        <v>169</v>
+        <v>171</v>
       </c>
       <c r="AX27">
         <v>73014</v>
@@ -5510,13 +5672,19 @@
       <c r="BH27">
         <v>0.0003355472814774799</v>
       </c>
+      <c r="BI27">
+        <v>32.2470703125</v>
+      </c>
+      <c r="BJ27">
+        <v>0.002535912298387097</v>
+      </c>
     </row>
-    <row r="28" spans="1:60">
+    <row r="28" spans="1:62">
       <c r="A28" s="1">
         <v>23</v>
       </c>
       <c r="B28" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="C28">
         <v>102.93543703505</v>
@@ -5549,7 +5717,7 @@
         <v>1.303336118142839</v>
       </c>
       <c r="M28" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="N28">
         <v>1388.264016264474</v>
@@ -5576,7 +5744,7 @@
         <v>1.186494600132325</v>
       </c>
       <c r="W28" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="X28">
         <v>1265.185801285288</v>
@@ -5615,16 +5783,16 @@
         <v>14.82261112007118</v>
       </c>
       <c r="AM28" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="AN28" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="AO28" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="AP28" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="AQ28">
         <v>27</v>
@@ -5639,10 +5807,10 @@
         <v>5</v>
       </c>
       <c r="AV28" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="AW28" t="s">
-        <v>170</v>
+        <v>172</v>
       </c>
       <c r="AX28">
         <v>73981</v>
@@ -5677,13 +5845,19 @@
       <c r="BH28">
         <v>0.0004024314351754541</v>
       </c>
+      <c r="BI28">
+        <v>32.0498046875</v>
+      </c>
+      <c r="BJ28">
+        <v>0.003091832797933997</v>
+      </c>
     </row>
-    <row r="29" spans="1:60">
+    <row r="29" spans="1:62">
       <c r="A29" s="1">
         <v>24</v>
       </c>
       <c r="B29" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="C29">
         <v>102.935654892051</v>
@@ -5716,7 +5890,7 @@
         <v>1.309225116511722</v>
       </c>
       <c r="M29" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="N29">
         <v>1388.256637755143</v>
@@ -5743,7 +5917,7 @@
         <v>1.181017537217525</v>
       </c>
       <c r="W29" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="X29">
         <v>1265.155657417724</v>
@@ -5773,16 +5947,16 @@
         <v>14.75460594781959</v>
       </c>
       <c r="AM29" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="AN29" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="AO29" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="AP29" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="AQ29">
         <v>27</v>
@@ -5797,10 +5971,10 @@
         <v>5</v>
       </c>
       <c r="AV29" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="AW29" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="AX29">
         <v>74262</v>
@@ -5835,13 +6009,19 @@
       <c r="BH29">
         <v>0.0003481433245195435</v>
       </c>
+      <c r="BI29">
+        <v>32.0908203125</v>
+      </c>
+      <c r="BJ29">
+        <v>0.001450108936004362</v>
+      </c>
     </row>
-    <row r="30" spans="1:60">
+    <row r="30" spans="1:62">
       <c r="A30" s="1">
         <v>25</v>
       </c>
       <c r="B30" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="C30">
         <v>102.9277296469321</v>
@@ -5874,7 +6054,7 @@
         <v>1.303376566078707</v>
       </c>
       <c r="M30" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="N30">
         <v>1388.263044421125</v>
@@ -5901,7 +6081,7 @@
         <v>1.158373048592429</v>
       </c>
       <c r="W30" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="X30">
         <v>1265.124641992391</v>
@@ -5940,16 +6120,16 @@
         <v>14.47314052761443</v>
       </c>
       <c r="AM30" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="AN30" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="AO30" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="AP30" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="AQ30">
         <v>27</v>
@@ -5964,10 +6144,10 @@
         <v>5</v>
       </c>
       <c r="AV30" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="AW30" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
       <c r="AX30">
         <v>74502</v>
@@ -6002,13 +6182,19 @@
       <c r="BH30">
         <v>0.0003122198518619767</v>
       </c>
+      <c r="BI30">
+        <v>32.1025390625</v>
+      </c>
+      <c r="BJ30">
+        <v>0.001015684051399009</v>
+      </c>
     </row>
-    <row r="31" spans="1:60">
+    <row r="31" spans="1:62">
       <c r="A31" s="1">
         <v>26</v>
       </c>
       <c r="B31" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="C31">
         <v>102.8013113858929</v>
@@ -6041,7 +6227,7 @@
         <v>1.145711337522244</v>
       </c>
       <c r="M31" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="N31">
         <v>1388.452124351453</v>
@@ -6068,7 +6254,7 @@
         <v>1.051108115993156</v>
       </c>
       <c r="W31" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="X31">
         <v>1265.457834486881</v>
@@ -6107,16 +6293,16 @@
         <v>13.12541579707171</v>
       </c>
       <c r="AM31" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="AN31" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="AO31" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="AP31" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="AQ31">
         <v>27</v>
@@ -6131,10 +6317,10 @@
         <v>5</v>
       </c>
       <c r="AV31" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="AW31" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="AX31">
         <v>74860</v>
@@ -6169,13 +6355,19 @@
       <c r="BH31">
         <v>0.001004291736518287</v>
       </c>
+      <c r="BI31">
+        <v>32.1005859375</v>
+      </c>
+      <c r="BJ31">
+        <v>0.0009464676030118749</v>
+      </c>
     </row>
-    <row r="32" spans="1:60">
+    <row r="32" spans="1:62">
       <c r="A32" s="1">
         <v>27</v>
       </c>
       <c r="B32" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="C32">
         <v>102.8035043508358</v>
@@ -6208,7 +6400,7 @@
         <v>1.143958809661653</v>
       </c>
       <c r="M32" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="N32">
         <v>1388.452240323286</v>
@@ -6235,7 +6427,7 @@
         <v>1.069319110236695</v>
       </c>
       <c r="W32" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="X32">
         <v>1265.423165271987</v>
@@ -6274,16 +6466,16 @@
         <v>13.35358949274716</v>
       </c>
       <c r="AM32" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="AN32" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="AO32" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="AP32" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="AQ32">
         <v>27</v>
@@ -6298,10 +6490,10 @@
         <v>5</v>
       </c>
       <c r="AV32" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="AW32" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="AX32">
         <v>75303</v>
@@ -6336,13 +6528,19 @@
       <c r="BH32">
         <v>0.0005259237791362568</v>
       </c>
+      <c r="BI32">
+        <v>32.115234375</v>
+      </c>
+      <c r="BJ32">
+        <v>0.001104043131059852</v>
+      </c>
     </row>
-    <row r="33" spans="1:60">
+    <row r="33" spans="1:62">
       <c r="A33" s="1">
         <v>28</v>
       </c>
       <c r="B33" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="C33">
         <v>102.8058161093926</v>
@@ -6375,7 +6573,7 @@
         <v>1.160147074700234</v>
       </c>
       <c r="M33" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="N33">
         <v>1388.453243315515</v>
@@ -6402,7 +6600,7 @@
         <v>1.070011637993247</v>
       </c>
       <c r="W33" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="X33">
         <v>1265.41882264024</v>
@@ -6441,16 +6639,16 @@
         <v>13.36227682697854</v>
       </c>
       <c r="AM33" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="AN33" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="AO33" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="AP33" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="AQ33">
         <v>27</v>
@@ -6465,10 +6663,10 @@
         <v>5</v>
       </c>
       <c r="AV33" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="AW33" t="s">
-        <v>175</v>
+        <v>177</v>
       </c>
       <c r="AX33">
         <v>75621</v>
@@ -6503,13 +6701,19 @@
       <c r="BH33">
         <v>0.0004690469467080387</v>
       </c>
+      <c r="BI33">
+        <v>32.1162109375</v>
+      </c>
+      <c r="BJ33">
+        <v>0.0008812056353878903</v>
+      </c>
     </row>
-    <row r="34" spans="1:60">
+    <row r="34" spans="1:62">
       <c r="A34" s="1">
         <v>0</v>
       </c>
       <c r="B34" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="C34">
         <v>102.7406649631779</v>
@@ -6542,7 +6746,7 @@
         <v>1.026758374146182</v>
       </c>
       <c r="M34" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="N34">
         <v>1388.582552756605</v>
@@ -6569,19 +6773,19 @@
         <v>1.01213137399856</v>
       </c>
       <c r="W34" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="AM34" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="AN34" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="AO34" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="AP34" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="AQ34">
         <v>27</v>
@@ -6596,10 +6800,10 @@
         <v>5</v>
       </c>
       <c r="AV34" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="AW34" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
       <c r="AX34">
         <v>76430</v>
@@ -6634,13 +6838,19 @@
       <c r="BH34">
         <v>0.0005296483401955726</v>
       </c>
+      <c r="BI34">
+        <v>32.119140625</v>
+      </c>
+      <c r="BJ34">
+        <v>0.001055875392982898</v>
+      </c>
     </row>
-    <row r="35" spans="1:60">
+    <row r="35" spans="1:62">
       <c r="A35" s="1">
         <v>1</v>
       </c>
       <c r="B35" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="C35">
         <v>102.7238024244249</v>
@@ -6673,7 +6883,7 @@
         <v>1.134907316805918</v>
       </c>
       <c r="M35" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="N35">
         <v>1388.582054345444</v>
@@ -6700,19 +6910,19 @@
         <v>0.9907071764681801</v>
       </c>
       <c r="W35" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="AM35" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="AN35" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="AO35" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="AP35" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="AQ35">
         <v>27</v>
@@ -6727,10 +6937,10 @@
         <v>5</v>
       </c>
       <c r="AV35" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="AW35" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
       <c r="AX35">
         <v>76859</v>
@@ -6765,13 +6975,19 @@
       <c r="BH35">
         <v>0.0004454446538975403</v>
       </c>
+      <c r="BI35">
+        <v>32.119140625</v>
+      </c>
+      <c r="BJ35">
+        <v>0.0009832145490892535</v>
+      </c>
     </row>
-    <row r="36" spans="1:60">
+    <row r="36" spans="1:62">
       <c r="A36" s="1">
         <v>2</v>
       </c>
       <c r="B36" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="C36">
         <v>102.692651437326</v>
@@ -6804,7 +7020,7 @@
         <v>1.205673403106951</v>
       </c>
       <c r="M36" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="N36">
         <v>1388.552095295028</v>
@@ -6831,19 +7047,19 @@
         <v>1.061162535726655</v>
       </c>
       <c r="W36" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="AM36" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="AN36" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="AO36" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="AP36" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="AQ36">
         <v>27</v>
@@ -6858,10 +7074,10 @@
         <v>5</v>
       </c>
       <c r="AV36" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="AW36" t="s">
-        <v>178</v>
+        <v>180</v>
       </c>
       <c r="AX36">
         <v>77508</v>
@@ -6896,13 +7112,19 @@
       <c r="BH36">
         <v>0.0004352950104070088</v>
       </c>
+      <c r="BI36">
+        <v>32.1083984375</v>
+      </c>
+      <c r="BJ36">
+        <v>0.003790113940693439</v>
+      </c>
     </row>
-    <row r="37" spans="1:60">
+    <row r="37" spans="1:62">
       <c r="A37" s="1">
         <v>3</v>
       </c>
       <c r="B37" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="C37">
         <v>104.523012613392</v>
@@ -6935,7 +7157,7 @@
         <v>1.195675976351994</v>
       </c>
       <c r="M37" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="N37">
         <v>1390.317555861073</v>
@@ -6962,19 +7184,19 @@
         <v>0.5064685504536746</v>
       </c>
       <c r="W37" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="AM37" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="AN37" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="AO37" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="AP37" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="AQ37">
         <v>27</v>
@@ -6989,10 +7211,10 @@
         <v>5</v>
       </c>
       <c r="AV37" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="AW37" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
       <c r="AX37">
         <v>77932</v>
@@ -7027,13 +7249,19 @@
       <c r="BH37">
         <v>0.000313263502440579</v>
       </c>
+      <c r="BI37">
+        <v>32.0830078125</v>
+      </c>
+      <c r="BJ37">
+        <v>0.002440547744951888</v>
+      </c>
     </row>
-    <row r="38" spans="1:60">
+    <row r="38" spans="1:62">
       <c r="A38" s="1">
         <v>4</v>
       </c>
       <c r="B38" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="C38">
         <v>102.7776570844861</v>
@@ -7066,7 +7294,7 @@
         <v>1.107518044252384</v>
       </c>
       <c r="M38" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="N38">
         <v>1388.533981280285</v>
@@ -7093,19 +7321,19 @@
         <v>1.09475834001511</v>
       </c>
       <c r="W38" t="s">
+        <v>99</v>
+      </c>
+      <c r="AM38" t="s">
         <v>97</v>
       </c>
-      <c r="AM38" t="s">
-        <v>95</v>
-      </c>
       <c r="AN38" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="AO38" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="AP38" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="AQ38">
         <v>27</v>
@@ -7120,10 +7348,10 @@
         <v>5</v>
       </c>
       <c r="AV38" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="AW38" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
       <c r="AX38">
         <v>78256</v>
@@ -7158,13 +7386,19 @@
       <c r="BH38">
         <v>0.0006304168721496208</v>
       </c>
+      <c r="BI38">
+        <v>32.06640625</v>
+      </c>
+      <c r="BJ38">
+        <v>0.001983198691992361</v>
+      </c>
     </row>
-    <row r="39" spans="1:60">
+    <row r="39" spans="1:62">
       <c r="A39" s="1">
         <v>5</v>
       </c>
       <c r="B39" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="C39">
         <v>102.7571581355663</v>
@@ -7197,7 +7431,7 @@
         <v>1.157639818752792</v>
       </c>
       <c r="M39" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="N39">
         <v>1388.545247738195</v>
@@ -7224,19 +7458,19 @@
         <v>1.064087082427681</v>
       </c>
       <c r="W39" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="AM39" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="AN39" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="AO39" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="AP39" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="AQ39">
         <v>27</v>
@@ -7251,10 +7485,10 @@
         <v>5</v>
       </c>
       <c r="AV39" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="AW39" t="s">
-        <v>181</v>
+        <v>183</v>
       </c>
       <c r="AX39">
         <v>78607</v>
@@ -7288,6 +7522,12 @@
       </c>
       <c r="BH39">
         <v>0.0004694369830851118</v>
+      </c>
+      <c r="BI39">
+        <v>32.0478515625</v>
+      </c>
+      <c r="BJ39">
+        <v>0.002123311327117022</v>
       </c>
     </row>
   </sheetData>

</xml_diff>